<commit_message>
improvements to the code FIX base.
</commit_message>
<xml_diff>
--- a/Mixed Fixture.xlsx
+++ b/Mixed Fixture.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Soheil\Desktop\projects\NSNTA-Timetable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F29317-39E2-4470-A5EE-30A852959616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDAD7F00-1F08-49AD-868A-EC4935F843C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4290" yWindow="480" windowWidth="20130" windowHeight="20520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31470" yWindow="480" windowWidth="20130" windowHeight="20520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="B Res 3" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>Hadfield</t>
   </si>
@@ -46,13 +46,10 @@
     <t>OLN</t>
   </si>
   <si>
-    <t>Home</t>
-  </si>
-  <si>
-    <t>Away</t>
-  </si>
-  <si>
     <t>Dates</t>
+  </si>
+  <si>
+    <t>Location</t>
   </si>
 </sst>
 </file>
@@ -448,182 +445,136 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13765F38-EF6D-47BF-9E70-9402D03C064B}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" style="7" customWidth="1"/>
     <col min="2" max="2" width="20" style="2" customWidth="1"/>
-    <col min="3" max="3" width="20.1640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>45875</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>45882</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>45889</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>45896</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>45903</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>45910</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>45917</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>45931</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>45938</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>45945</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>45952</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <v>45959</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>45966</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <v>45973</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>